<commit_message>
made excecises of chapter 25 and 26
</commit_message>
<xml_diff>
--- a/Overzicht.xlsx
+++ b/Overzicht.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
@@ -52,7 +52,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -62,12 +62,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -84,14 +78,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -107,9 +100,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kantoor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -147,9 +140,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kantoor">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,7 +177,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -219,7 +212,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kantoor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -396,7 +389,7 @@
   <dimension ref="B3:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G6" sqref="G6:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,7 +456,7 @@
       <c r="F5">
         <v>18</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="1">
         <v>24</v>
       </c>
       <c r="H5">
@@ -486,7 +479,7 @@
       <c r="F6">
         <v>19</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="1">
         <v>25</v>
       </c>
       <c r="H6">
@@ -504,7 +497,7 @@
       <c r="F7" s="1">
         <v>21</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="1">
         <v>26</v>
       </c>
       <c r="H7">

</xml_diff>